<commit_message>
created updated better asset finish tomorrow
</commit_message>
<xml_diff>
--- a/examples/20242 Monitor for Mannyresults.xlsx
+++ b/examples/20242 Monitor for Mannyresults.xlsx
@@ -53,7 +53,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -254,116 +254,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="00000000"/>
-      </left>
-      <top style="medium">
-        <color rgb="00000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="00000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="medium">
-        <color rgb="00000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="00000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="00000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="00000000"/>
-      </left>
-      <top style="medium">
-        <color rgb="00000000"/>
-      </top>
-    </border>
-    <border>
-      <top style="medium">
-        <color rgb="00000000"/>
-      </top>
-    </border>
-    <border>
-      <right style="medium">
-        <color rgb="00000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="00000000"/>
-      </top>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="00000000"/>
-      </left>
-      <bottom style="medium">
-        <color rgb="00000000"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="medium">
-        <color rgb="00000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="medium">
-        <color rgb="00000000"/>
-      </right>
-      <bottom style="medium">
-        <color rgb="00000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="00000000"/>
-      </left>
-    </border>
-    <border/>
-    <border>
-      <right style="medium">
-        <color rgb="00000000"/>
-      </right>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="00000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="00000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="00000000"/>
-      </top>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="00000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="00000000"/>
-      </right>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="00000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="00000000"/>
-      </right>
-      <bottom style="medium">
-        <color rgb="00000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -497,41 +392,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -988,15 +849,13 @@
     <col width="3.140625" customWidth="1" style="5" min="45" max="45"/>
     <col width="9.7109375" customWidth="1" style="5" min="46" max="46"/>
     <col width="6.42578125" customWidth="1" style="5" min="47" max="47"/>
-    <col width="2.43" customWidth="1" style="5" min="48" max="48"/>
-    <col width="9" customWidth="1" style="5" min="49" max="49"/>
-    <col width="6" customWidth="1" style="5" min="50" max="50"/>
-    <col width="1.86" customWidth="1" style="5" min="51" max="51"/>
-    <col width="2.57" customWidth="1" style="5" min="52" max="52"/>
-    <col width="9.289999999999999" customWidth="1" style="5" min="53" max="53"/>
-    <col width="1.86" customWidth="1" style="5" min="54" max="16384"/>
-    <col width="2.57" customWidth="1" min="55" max="55"/>
-    <col width="9.289999999999999" customWidth="1" min="56" max="56"/>
+    <col width="2.5703125" customWidth="1" style="5" min="48" max="48"/>
+    <col width="3.28515625" customWidth="1" style="5" min="49" max="49"/>
+    <col width="10" customWidth="1" style="5" min="50" max="50"/>
+    <col width="2.5703125" customWidth="1" style="5" min="51" max="51"/>
+    <col width="3.28515625" customWidth="1" style="5" min="52" max="52"/>
+    <col width="10" customWidth="1" style="5" min="53" max="53"/>
+    <col width="9.140625" customWidth="1" style="5" min="54" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -1079,13 +938,6 @@
         <v>44774</v>
       </c>
       <c r="AU1" s="48" t="n"/>
-      <c r="AV1" s="49" t="n"/>
-      <c r="AW1" s="50" t="inlineStr">
-        <is>
-          <t>2023/03/19</t>
-        </is>
-      </c>
-      <c r="AX1" s="51" t="n"/>
       <c r="AY1" s="15" t="n"/>
       <c r="AZ1" s="47" t="inlineStr">
         <is>
@@ -1111,13 +963,13 @@
           <t>Location</t>
         </is>
       </c>
-      <c r="C2" s="52" t="n"/>
+      <c r="C2" s="49" t="n"/>
       <c r="D2" s="8" t="inlineStr">
         <is>
           <t>Location</t>
         </is>
       </c>
-      <c r="E2" s="52" t="n"/>
+      <c r="E2" s="49" t="n"/>
       <c r="F2" s="12" t="n"/>
       <c r="G2" s="25" t="inlineStr">
         <is>
@@ -1272,30 +1124,19 @@
           <t>Delta</t>
         </is>
       </c>
-      <c r="AV2" s="53" t="n"/>
-      <c r="AW2" s="54" t="inlineStr">
-        <is>
-          <t>Location</t>
-        </is>
-      </c>
-      <c r="AX2" s="55" t="inlineStr">
-        <is>
-          <t>Delta</t>
-        </is>
-      </c>
       <c r="AY2" s="6" t="n"/>
       <c r="AZ2" s="8" t="inlineStr">
         <is>
           <t>Delta (feet)</t>
         </is>
       </c>
-      <c r="BA2" s="52" t="n"/>
+      <c r="BA2" s="49" t="n"/>
       <c r="BC2" s="8" t="inlineStr">
         <is>
           <t>Delta (inches)</t>
         </is>
       </c>
-      <c r="BD2" s="52" t="n"/>
+      <c r="BD2" s="49" t="n"/>
     </row>
     <row r="3" hidden="1" ht="12.75" customHeight="1">
       <c r="A3" s="4" t="n">
@@ -1485,39 +1326,35 @@
         <f>AT3-AP3</f>
         <v/>
       </c>
-      <c r="AV3" s="49" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="AW3" s="56" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="AX3" s="57" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="AY3" s="20" t="n"/>
+      <c r="AV3" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AW3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY3" s="14" t="n"/>
       <c r="AZ3" s="10" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="BA3" s="17" t="n">
-        <v>0</v>
-      </c>
+      <c r="BA3" s="17" t="n"/>
       <c r="BB3" s="14" t="n"/>
       <c r="BC3" s="10" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="BD3" s="17" t="n">
-        <v>0</v>
-      </c>
+      <c r="BD3" s="17" t="n"/>
     </row>
     <row r="4" hidden="1" ht="12.75" customHeight="1">
       <c r="A4" s="4" t="n"/>
@@ -1705,39 +1542,35 @@
         <f>AT4-AP4</f>
         <v/>
       </c>
-      <c r="AV4" s="58" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="AW4" s="59" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="AX4" s="60" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="AY4" s="20" t="n"/>
+      <c r="AV4" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="AW4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY4" s="14" t="n"/>
       <c r="AZ4" s="10" t="inlineStr">
         <is>
           <t>E</t>
         </is>
       </c>
-      <c r="BA4" s="17" t="n">
-        <v>0</v>
-      </c>
+      <c r="BA4" s="17" t="n"/>
       <c r="BB4" s="14" t="n"/>
       <c r="BC4" s="10" t="inlineStr">
         <is>
           <t>E</t>
         </is>
       </c>
-      <c r="BD4" s="17" t="n">
-        <v>0</v>
-      </c>
+      <c r="BD4" s="17" t="n"/>
     </row>
     <row r="5" hidden="1" ht="12.75" customHeight="1">
       <c r="A5" s="3" t="n"/>
@@ -1925,39 +1758,35 @@
         <f>AT5-AP5</f>
         <v/>
       </c>
-      <c r="AV5" s="53" t="inlineStr">
-        <is>
-          <t>EL</t>
-        </is>
-      </c>
-      <c r="AW5" s="61" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="AX5" s="62" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="AY5" s="20" t="n"/>
+      <c r="AV5" t="inlineStr">
+        <is>
+          <t>EL</t>
+        </is>
+      </c>
+      <c r="AW5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY5" s="14" t="n"/>
       <c r="AZ5" s="11" t="inlineStr">
         <is>
           <t>EL</t>
         </is>
       </c>
-      <c r="BA5" s="24" t="n">
-        <v>0</v>
-      </c>
+      <c r="BA5" s="24" t="n"/>
       <c r="BB5" s="14" t="n"/>
       <c r="BC5" s="11" t="inlineStr">
         <is>
           <t>EL</t>
         </is>
       </c>
-      <c r="BD5" s="24" t="n">
-        <v>0</v>
-      </c>
+      <c r="BD5" s="24" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="4" t="n">
@@ -2153,27 +1982,30 @@
         <f>AT6-AQ6</f>
         <v/>
       </c>
-      <c r="AV6" s="49" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="AW6" s="56" t="inlineStr">
-        <is>
-          <t>2116934.780</t>
-        </is>
-      </c>
-      <c r="AX6" s="57" t="n">
-        <v>2110000</v>
-      </c>
-      <c r="AY6" s="20" t="n"/>
+      <c r="AV6" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AW6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY6" s="14" t="n"/>
       <c r="AZ6" s="10" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="BA6" s="17" t="n">
-        <v>2110000.008</v>
+      <c r="BA6" s="17">
+        <f>AT6-E6</f>
+        <v/>
       </c>
       <c r="BB6" s="14" t="n"/>
       <c r="BC6" s="10" t="inlineStr">
@@ -2181,8 +2013,9 @@
           <t>N</t>
         </is>
       </c>
-      <c r="BD6" s="13" t="n">
-        <v>25320000.1</v>
+      <c r="BD6" s="13">
+        <f>AX6*12</f>
+        <v/>
       </c>
     </row>
     <row r="7">
@@ -2377,27 +2210,30 @@
         <f>AT7-AQ7</f>
         <v/>
       </c>
-      <c r="AV7" s="58" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="AW7" s="59" t="inlineStr">
-        <is>
-          <t>6114496.237</t>
-        </is>
-      </c>
-      <c r="AX7" s="60" t="n">
-        <v>6110000</v>
-      </c>
-      <c r="AY7" s="20" t="n"/>
+      <c r="AV7" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="AW7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY7" s="14" t="n"/>
       <c r="AZ7" s="10" t="inlineStr">
         <is>
           <t>E</t>
         </is>
       </c>
-      <c r="BA7" s="17" t="n">
-        <v>6110000.004</v>
+      <c r="BA7" s="17">
+        <f>AT7-E7</f>
+        <v/>
       </c>
       <c r="BB7" s="14" t="n"/>
       <c r="BC7" s="10" t="inlineStr">
@@ -2405,8 +2241,9 @@
           <t>E</t>
         </is>
       </c>
-      <c r="BD7" s="13" t="n">
-        <v>73320000.05</v>
+      <c r="BD7" s="13">
+        <f>AX7*12</f>
+        <v/>
       </c>
     </row>
     <row r="8">
@@ -2601,27 +2438,30 @@
         <f>AT8-AQ8</f>
         <v/>
       </c>
-      <c r="AV8" s="53" t="inlineStr">
-        <is>
-          <t>EL</t>
-        </is>
-      </c>
-      <c r="AW8" s="61" t="inlineStr">
-        <is>
-          <t>45.767</t>
-        </is>
-      </c>
-      <c r="AX8" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY8" s="20" t="n"/>
+      <c r="AV8" t="inlineStr">
+        <is>
+          <t>EL</t>
+        </is>
+      </c>
+      <c r="AW8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY8" s="14" t="n"/>
       <c r="AZ8" s="11" t="inlineStr">
         <is>
           <t>EL</t>
         </is>
       </c>
-      <c r="BA8" s="24" t="n">
-        <v>0.006</v>
+      <c r="BA8" s="24">
+        <f>AT8-E8</f>
+        <v/>
       </c>
       <c r="BB8" s="14" t="n"/>
       <c r="BC8" s="11" t="inlineStr">
@@ -2629,8 +2469,9 @@
           <t>EL</t>
         </is>
       </c>
-      <c r="BD8" s="29" t="n">
-        <v>0.07000000000000001</v>
+      <c r="BD8" s="29">
+        <f>AX8*12</f>
+        <v/>
       </c>
     </row>
     <row r="9">
@@ -2821,27 +2662,30 @@
         <f>AT9-AQ9</f>
         <v/>
       </c>
-      <c r="AV9" s="49" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="AW9" s="56" t="inlineStr">
-        <is>
-          <t>2116916.329</t>
-        </is>
-      </c>
-      <c r="AX9" s="57" t="n">
-        <v>2110000</v>
-      </c>
-      <c r="AY9" s="20" t="n"/>
+      <c r="AV9" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AW9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX9" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY9" s="14" t="n"/>
       <c r="AZ9" s="10" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="BA9" s="17" t="n">
-        <v>2110000.026</v>
+      <c r="BA9" s="17">
+        <f>AT9-E9</f>
+        <v/>
       </c>
       <c r="BB9" s="14" t="n"/>
       <c r="BC9" s="10" t="inlineStr">
@@ -2849,8 +2693,9 @@
           <t>N</t>
         </is>
       </c>
-      <c r="BD9" s="13" t="n">
-        <v>25320000.31</v>
+      <c r="BD9" s="13">
+        <f>AX9*12</f>
+        <v/>
       </c>
     </row>
     <row r="10">
@@ -3039,27 +2884,30 @@
         <f>AT10-AQ10</f>
         <v/>
       </c>
-      <c r="AV10" s="58" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="AW10" s="59" t="inlineStr">
-        <is>
-          <t>6114462.796</t>
-        </is>
-      </c>
-      <c r="AX10" s="60" t="n">
-        <v>6110000</v>
-      </c>
-      <c r="AY10" s="20" t="n"/>
+      <c r="AV10" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="AW10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX10" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY10" s="14" t="n"/>
       <c r="AZ10" s="10" t="inlineStr">
         <is>
           <t>E</t>
         </is>
       </c>
-      <c r="BA10" s="17" t="n">
-        <v>6109999.992</v>
+      <c r="BA10" s="17">
+        <f>AT10-E10</f>
+        <v/>
       </c>
       <c r="BB10" s="14" t="n"/>
       <c r="BC10" s="10" t="inlineStr">
@@ -3067,8 +2915,9 @@
           <t>E</t>
         </is>
       </c>
-      <c r="BD10" s="13" t="n">
-        <v>73319999.90000001</v>
+      <c r="BD10" s="13">
+        <f>AX10*12</f>
+        <v/>
       </c>
     </row>
     <row r="11">
@@ -3257,27 +3106,30 @@
         <f>AT11-AQ11</f>
         <v/>
       </c>
-      <c r="AV11" s="53" t="inlineStr">
-        <is>
-          <t>EL</t>
-        </is>
-      </c>
-      <c r="AW11" s="61" t="inlineStr">
-        <is>
-          <t>45.813</t>
-        </is>
-      </c>
-      <c r="AX11" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY11" s="20" t="n"/>
+      <c r="AV11" t="inlineStr">
+        <is>
+          <t>EL</t>
+        </is>
+      </c>
+      <c r="AW11" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX11" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY11" s="14" t="n"/>
       <c r="AZ11" s="11" t="inlineStr">
         <is>
           <t>EL</t>
         </is>
       </c>
-      <c r="BA11" s="24" t="n">
-        <v>0.012</v>
+      <c r="BA11" s="24">
+        <f>AT11-E11</f>
+        <v/>
       </c>
       <c r="BB11" s="14" t="n"/>
       <c r="BC11" s="11" t="inlineStr">
@@ -3285,8 +3137,9 @@
           <t>EL</t>
         </is>
       </c>
-      <c r="BD11" s="29" t="n">
-        <v>0.14</v>
+      <c r="BD11" s="29">
+        <f>AX11*12</f>
+        <v/>
       </c>
     </row>
     <row r="12">
@@ -3477,27 +3330,30 @@
         <f>AT12-AQ12</f>
         <v/>
       </c>
-      <c r="AV12" s="49" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="AW12" s="56" t="inlineStr">
-        <is>
-          <t>2116893.420</t>
-        </is>
-      </c>
-      <c r="AX12" s="57" t="n">
-        <v>2110000</v>
-      </c>
-      <c r="AY12" s="20" t="n"/>
+      <c r="AV12" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AW12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX12" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY12" s="14" t="n"/>
       <c r="AZ12" s="10" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="BA12" s="17" t="n">
-        <v>2109999.997</v>
+      <c r="BA12" s="17">
+        <f>AT12-E12</f>
+        <v/>
       </c>
       <c r="BB12" s="14" t="n"/>
       <c r="BC12" s="10" t="inlineStr">
@@ -3505,8 +3361,9 @@
           <t>N</t>
         </is>
       </c>
-      <c r="BD12" s="13" t="n">
-        <v>25319999.96</v>
+      <c r="BD12" s="13">
+        <f>AX12*12</f>
+        <v/>
       </c>
     </row>
     <row r="13">
@@ -3695,27 +3552,30 @@
         <f>AT13-AQ13</f>
         <v/>
       </c>
-      <c r="AV13" s="58" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="AW13" s="59" t="inlineStr">
-        <is>
-          <t>6114421.504</t>
-        </is>
-      </c>
-      <c r="AX13" s="60" t="n">
-        <v>6110000</v>
-      </c>
-      <c r="AY13" s="20" t="n"/>
+      <c r="AV13" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="AW13" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX13" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY13" s="14" t="n"/>
       <c r="AZ13" s="10" t="inlineStr">
         <is>
           <t>E</t>
         </is>
       </c>
-      <c r="BA13" s="17" t="n">
-        <v>6110000.003</v>
+      <c r="BA13" s="17">
+        <f>AT13-E13</f>
+        <v/>
       </c>
       <c r="BB13" s="14" t="n"/>
       <c r="BC13" s="10" t="inlineStr">
@@ -3723,8 +3583,9 @@
           <t>E</t>
         </is>
       </c>
-      <c r="BD13" s="13" t="n">
-        <v>73320000.04000001</v>
+      <c r="BD13" s="13">
+        <f>AX13*12</f>
+        <v/>
       </c>
     </row>
     <row r="14">
@@ -3913,27 +3774,30 @@
         <f>AT14-AQ14</f>
         <v/>
       </c>
-      <c r="AV14" s="53" t="inlineStr">
-        <is>
-          <t>EL</t>
-        </is>
-      </c>
-      <c r="AW14" s="61" t="inlineStr">
-        <is>
-          <t>43.614</t>
-        </is>
-      </c>
-      <c r="AX14" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY14" s="20" t="n"/>
+      <c r="AV14" t="inlineStr">
+        <is>
+          <t>EL</t>
+        </is>
+      </c>
+      <c r="AW14" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX14" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY14" s="14" t="n"/>
       <c r="AZ14" s="11" t="inlineStr">
         <is>
           <t>EL</t>
         </is>
       </c>
-      <c r="BA14" s="24" t="n">
-        <v>0.01</v>
+      <c r="BA14" s="24">
+        <f>AT14-E14</f>
+        <v/>
       </c>
       <c r="BB14" s="14" t="n"/>
       <c r="BC14" s="11" t="inlineStr">
@@ -3941,8 +3805,9 @@
           <t>EL</t>
         </is>
       </c>
-      <c r="BD14" s="29" t="n">
-        <v>0.12</v>
+      <c r="BD14" s="29">
+        <f>AX14*12</f>
+        <v/>
       </c>
     </row>
     <row r="15">
@@ -4145,27 +4010,30 @@
         <f>AT15-AQ15</f>
         <v/>
       </c>
-      <c r="AV15" s="49" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="AW15" s="56" t="inlineStr">
-        <is>
-          <t>2116964.026</t>
-        </is>
-      </c>
-      <c r="AX15" s="57" t="n">
-        <v>2110000</v>
-      </c>
-      <c r="AY15" s="20" t="n"/>
+      <c r="AV15" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AW15" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX15" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY15" s="14" t="n"/>
       <c r="AZ15" s="10" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="BA15" s="17" t="n">
-        <v>2109999.999</v>
+      <c r="BA15" s="17">
+        <f>AT15-E15</f>
+        <v/>
       </c>
       <c r="BB15" s="14" t="n"/>
       <c r="BC15" s="10" t="inlineStr">
@@ -4173,8 +4041,9 @@
           <t>N</t>
         </is>
       </c>
-      <c r="BD15" s="13" t="n">
-        <v>25319999.99</v>
+      <c r="BD15" s="13">
+        <f>AX15*12</f>
+        <v/>
       </c>
     </row>
     <row r="16">
@@ -4379,27 +4248,30 @@
         <f>AT16-AQ16</f>
         <v/>
       </c>
-      <c r="AV16" s="58" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="AW16" s="59" t="inlineStr">
-        <is>
-          <t>6114405.002</t>
-        </is>
-      </c>
-      <c r="AX16" s="60" t="n">
-        <v>6110000</v>
-      </c>
-      <c r="AY16" s="20" t="n"/>
+      <c r="AV16" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="AW16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX16" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY16" s="14" t="n"/>
       <c r="AZ16" s="10" t="inlineStr">
         <is>
           <t>E</t>
         </is>
       </c>
-      <c r="BA16" s="17" t="n">
-        <v>6110000.009</v>
+      <c r="BA16" s="17">
+        <f>AT16-E16</f>
+        <v/>
       </c>
       <c r="BB16" s="14" t="n"/>
       <c r="BC16" s="10" t="inlineStr">
@@ -4407,8 +4279,9 @@
           <t>E</t>
         </is>
       </c>
-      <c r="BD16" s="13" t="n">
-        <v>73320000.11</v>
+      <c r="BD16" s="13">
+        <f>AX16*12</f>
+        <v/>
       </c>
     </row>
     <row r="17">
@@ -4609,27 +4482,30 @@
         <f>AT17-AQ17</f>
         <v/>
       </c>
-      <c r="AV17" s="53" t="inlineStr">
-        <is>
-          <t>EL</t>
-        </is>
-      </c>
-      <c r="AW17" s="61" t="inlineStr">
-        <is>
-          <t>44.538</t>
-        </is>
-      </c>
-      <c r="AX17" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY17" s="20" t="n"/>
+      <c r="AV17" t="inlineStr">
+        <is>
+          <t>EL</t>
+        </is>
+      </c>
+      <c r="AW17" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX17" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY17" s="14" t="n"/>
       <c r="AZ17" s="11" t="inlineStr">
         <is>
           <t>EL</t>
         </is>
       </c>
-      <c r="BA17" s="24" t="n">
-        <v>0.012</v>
+      <c r="BA17" s="24">
+        <f>AT17-E17</f>
+        <v/>
       </c>
       <c r="BB17" s="14" t="n"/>
       <c r="BC17" s="11" t="inlineStr">
@@ -4637,8 +4513,9 @@
           <t>EL</t>
         </is>
       </c>
-      <c r="BD17" s="29" t="n">
-        <v>0.14</v>
+      <c r="BD17" s="29">
+        <f>AX17*12</f>
+        <v/>
       </c>
     </row>
     <row r="18">
@@ -4841,27 +4718,30 @@
         <f>AT18-AQ18</f>
         <v/>
       </c>
-      <c r="AV18" s="49" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="AW18" s="56" t="inlineStr">
-        <is>
-          <t>2116981.294</t>
-        </is>
-      </c>
-      <c r="AX18" s="57" t="n">
-        <v>2110000</v>
-      </c>
-      <c r="AY18" s="20" t="n"/>
+      <c r="AV18" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AW18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX18" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY18" s="14" t="n"/>
       <c r="AZ18" s="10" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="BA18" s="17" t="n">
-        <v>2109999.977</v>
+      <c r="BA18" s="17">
+        <f>AT18-E18</f>
+        <v/>
       </c>
       <c r="BB18" s="14" t="n"/>
       <c r="BC18" s="10" t="inlineStr">
@@ -4869,8 +4749,9 @@
           <t>N</t>
         </is>
       </c>
-      <c r="BD18" s="13" t="n">
-        <v>25319999.72</v>
+      <c r="BD18" s="13">
+        <f>AX18*12</f>
+        <v/>
       </c>
     </row>
     <row r="19">
@@ -5071,27 +4952,30 @@
         <f>AT19-AQ19</f>
         <v/>
       </c>
-      <c r="AV19" s="58" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="AW19" s="59" t="inlineStr">
-        <is>
-          <t>6114435.931</t>
-        </is>
-      </c>
-      <c r="AX19" s="60" t="n">
-        <v>6110000</v>
-      </c>
-      <c r="AY19" s="20" t="n"/>
+      <c r="AV19" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="AW19" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX19" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY19" s="5" t="n"/>
       <c r="AZ19" s="10" t="inlineStr">
         <is>
           <t>E</t>
         </is>
       </c>
-      <c r="BA19" s="17" t="n">
-        <v>6110000.016</v>
+      <c r="BA19" s="17">
+        <f>AT19-E19</f>
+        <v/>
       </c>
       <c r="BB19" s="5" t="n"/>
       <c r="BC19" s="10" t="inlineStr">
@@ -5099,8 +4983,9 @@
           <t>E</t>
         </is>
       </c>
-      <c r="BD19" s="13" t="n">
-        <v>73320000.19</v>
+      <c r="BD19" s="13">
+        <f>AX19*12</f>
+        <v/>
       </c>
     </row>
     <row r="20">
@@ -5301,27 +5186,30 @@
         <f>AT20-AQ20</f>
         <v/>
       </c>
-      <c r="AV20" s="53" t="inlineStr">
-        <is>
-          <t>EL</t>
-        </is>
-      </c>
-      <c r="AW20" s="61" t="inlineStr">
-        <is>
-          <t>44.782</t>
-        </is>
-      </c>
-      <c r="AX20" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY20" s="20" t="n"/>
+      <c r="AV20" t="inlineStr">
+        <is>
+          <t>EL</t>
+        </is>
+      </c>
+      <c r="AW20" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX20" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY20" s="5" t="n"/>
       <c r="AZ20" s="11" t="inlineStr">
         <is>
           <t>EL</t>
         </is>
       </c>
-      <c r="BA20" s="24" t="n">
-        <v>0.012</v>
+      <c r="BA20" s="24">
+        <f>AT20-E20</f>
+        <v/>
       </c>
       <c r="BB20" s="5" t="n"/>
       <c r="BC20" s="11" t="inlineStr">
@@ -5329,8 +5217,9 @@
           <t>EL</t>
         </is>
       </c>
-      <c r="BD20" s="29" t="n">
-        <v>0.14</v>
+      <c r="BD20" s="29">
+        <f>AX20*12</f>
+        <v/>
       </c>
     </row>
     <row r="21">
@@ -5539,29 +5428,30 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="AV21" s="49" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="AW21" s="56" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="AX21" s="57" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="AY21" s="20" t="n"/>
+      <c r="AV21" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AW21" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX21" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY21" s="5" t="n"/>
       <c r="AZ21" s="10" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="BA21" s="17" t="n">
-        <v>-0.003</v>
+      <c r="BA21" s="17">
+        <f>AE21-E21</f>
+        <v/>
       </c>
       <c r="BB21" s="5" t="n"/>
       <c r="BC21" s="10" t="inlineStr">
@@ -5569,8 +5459,9 @@
           <t>N</t>
         </is>
       </c>
-      <c r="BD21" s="13" t="n">
-        <v>-0.04</v>
+      <c r="BD21" s="13">
+        <f>AX21*12</f>
+        <v/>
       </c>
     </row>
     <row r="22">
@@ -5777,29 +5668,30 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="AV22" s="58" t="inlineStr">
-        <is>
-          <t>E</t>
-        </is>
-      </c>
-      <c r="AW22" s="59" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="AX22" s="60" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="AY22" s="20" t="n"/>
+      <c r="AV22" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="AW22" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX22" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY22" s="5" t="n"/>
       <c r="AZ22" s="10" t="inlineStr">
         <is>
           <t>E</t>
         </is>
       </c>
-      <c r="BA22" s="17" t="n">
-        <v>0.005</v>
+      <c r="BA22" s="17">
+        <f>AE22-E22</f>
+        <v/>
       </c>
       <c r="BB22" s="5" t="n"/>
       <c r="BC22" s="10" t="inlineStr">
@@ -5807,8 +5699,9 @@
           <t>E</t>
         </is>
       </c>
-      <c r="BD22" s="13" t="n">
-        <v>0.06</v>
+      <c r="BD22" s="13">
+        <f>AX22*12</f>
+        <v/>
       </c>
     </row>
     <row r="23">
@@ -6015,29 +5908,30 @@
           <t>NA</t>
         </is>
       </c>
-      <c r="AV23" s="53" t="inlineStr">
-        <is>
-          <t>EL</t>
-        </is>
-      </c>
-      <c r="AW23" s="61" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="AX23" s="62" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="AY23" s="20" t="n"/>
+      <c r="AV23" t="inlineStr">
+        <is>
+          <t>EL</t>
+        </is>
+      </c>
+      <c r="AW23" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AX23" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY23" s="5" t="n"/>
       <c r="AZ23" s="11" t="inlineStr">
         <is>
           <t>EL</t>
         </is>
       </c>
-      <c r="BA23" s="24" t="n">
-        <v>0.003</v>
+      <c r="BA23" s="24">
+        <f>AE23-E23</f>
+        <v/>
       </c>
       <c r="BB23" s="5" t="n"/>
       <c r="BC23" s="11" t="inlineStr">
@@ -6045,8 +5939,9 @@
           <t>EL</t>
         </is>
       </c>
-      <c r="BD23" s="29" t="n">
-        <v>0.04</v>
+      <c r="BD23" s="29">
+        <f>AX23*12</f>
+        <v/>
       </c>
     </row>
     <row r="24">
@@ -6163,10 +6058,22 @@
       </c>
       <c r="AT24" s="17" t="n"/>
       <c r="AU24" s="23" t="n"/>
-      <c r="AV24" s="49" t="n"/>
-      <c r="AW24" s="56" t="n"/>
-      <c r="AX24" s="57" t="n"/>
-      <c r="AY24" s="20" t="n"/>
+      <c r="AV24" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AW24" t="inlineStr">
+        <is>
+          <t>9889.979</t>
+        </is>
+      </c>
+      <c r="AX24" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY24" s="5" t="n"/>
       <c r="AZ24" s="10" t="inlineStr">
         <is>
           <t>N</t>
@@ -6295,10 +6202,22 @@
       </c>
       <c r="AT25" s="18" t="n"/>
       <c r="AU25" s="17" t="n"/>
-      <c r="AV25" s="58" t="n"/>
-      <c r="AW25" s="59" t="n"/>
-      <c r="AX25" s="60" t="n"/>
-      <c r="AY25" s="20" t="n"/>
+      <c r="AV25" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="AW25" t="inlineStr">
+        <is>
+          <t>9977.973</t>
+        </is>
+      </c>
+      <c r="AX25" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY25" s="5" t="n"/>
       <c r="AZ25" s="10" t="inlineStr">
         <is>
           <t>E</t>
@@ -6427,10 +6346,22 @@
       </c>
       <c r="AT26" s="21" t="n"/>
       <c r="AU26" s="17" t="n"/>
-      <c r="AV26" s="53" t="n"/>
-      <c r="AW26" s="61" t="n"/>
-      <c r="AX26" s="62" t="n"/>
-      <c r="AY26" s="20" t="n"/>
+      <c r="AV26" t="inlineStr">
+        <is>
+          <t>EL</t>
+        </is>
+      </c>
+      <c r="AW26" t="inlineStr">
+        <is>
+          <t>17.405</t>
+        </is>
+      </c>
+      <c r="AX26" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY26" s="5" t="n"/>
       <c r="AZ26" s="11" t="inlineStr">
         <is>
           <t>EL</t>
@@ -6559,10 +6490,22 @@
       </c>
       <c r="AT27" s="17" t="n"/>
       <c r="AU27" s="16" t="n"/>
-      <c r="AV27" s="49" t="n"/>
-      <c r="AW27" s="56" t="n"/>
-      <c r="AX27" s="57" t="n"/>
-      <c r="AY27" s="20" t="n"/>
+      <c r="AV27" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AW27" t="inlineStr">
+        <is>
+          <t>9889.979</t>
+        </is>
+      </c>
+      <c r="AX27" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY27" s="5" t="n"/>
       <c r="AZ27" s="10" t="inlineStr">
         <is>
           <t>N</t>
@@ -6691,10 +6634,22 @@
       </c>
       <c r="AT28" s="18" t="n"/>
       <c r="AU28" s="13" t="n"/>
-      <c r="AV28" s="58" t="n"/>
-      <c r="AW28" s="59" t="n"/>
-      <c r="AX28" s="60" t="n"/>
-      <c r="AY28" s="20" t="n"/>
+      <c r="AV28" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="AW28" t="inlineStr">
+        <is>
+          <t>9977.973</t>
+        </is>
+      </c>
+      <c r="AX28" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY28" s="5" t="n"/>
       <c r="AZ28" s="10" t="inlineStr">
         <is>
           <t>E</t>
@@ -6823,10 +6778,22 @@
       </c>
       <c r="AT29" s="21" t="n"/>
       <c r="AU29" s="13" t="n"/>
-      <c r="AV29" s="53" t="n"/>
-      <c r="AW29" s="61" t="n"/>
-      <c r="AX29" s="62" t="n"/>
-      <c r="AY29" s="20" t="n"/>
+      <c r="AV29" t="inlineStr">
+        <is>
+          <t>EL</t>
+        </is>
+      </c>
+      <c r="AW29" t="inlineStr">
+        <is>
+          <t>17.405</t>
+        </is>
+      </c>
+      <c r="AX29" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY29" s="5" t="n"/>
       <c r="AZ29" s="11" t="inlineStr">
         <is>
           <t>EL</t>
@@ -6955,10 +6922,22 @@
       </c>
       <c r="AT30" s="17" t="n"/>
       <c r="AU30" s="23" t="n"/>
-      <c r="AV30" s="49" t="n"/>
-      <c r="AW30" s="56" t="n"/>
-      <c r="AX30" s="57" t="n"/>
-      <c r="AY30" s="20" t="n"/>
+      <c r="AV30" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AW30" t="inlineStr">
+        <is>
+          <t>9889.979</t>
+        </is>
+      </c>
+      <c r="AX30" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY30" s="5" t="n"/>
       <c r="AZ30" s="10" t="inlineStr">
         <is>
           <t>N</t>
@@ -7087,10 +7066,22 @@
       </c>
       <c r="AT31" s="18" t="n"/>
       <c r="AU31" s="17" t="n"/>
-      <c r="AV31" s="58" t="n"/>
-      <c r="AW31" s="59" t="n"/>
-      <c r="AX31" s="60" t="n"/>
-      <c r="AY31" s="20" t="n"/>
+      <c r="AV31" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="AW31" t="inlineStr">
+        <is>
+          <t>9977.973</t>
+        </is>
+      </c>
+      <c r="AX31" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY31" s="5" t="n"/>
       <c r="AZ31" s="10" t="inlineStr">
         <is>
           <t>E</t>
@@ -7219,10 +7210,22 @@
       </c>
       <c r="AT32" s="21" t="n"/>
       <c r="AU32" s="17" t="n"/>
-      <c r="AV32" s="53" t="n"/>
-      <c r="AW32" s="61" t="n"/>
-      <c r="AX32" s="62" t="n"/>
-      <c r="AY32" s="20" t="n"/>
+      <c r="AV32" t="inlineStr">
+        <is>
+          <t>EL</t>
+        </is>
+      </c>
+      <c r="AW32" t="inlineStr">
+        <is>
+          <t>17.405</t>
+        </is>
+      </c>
+      <c r="AX32" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY32" s="5" t="n"/>
       <c r="AZ32" s="11" t="inlineStr">
         <is>
           <t>EL</t>
@@ -7351,10 +7354,22 @@
       </c>
       <c r="AT33" s="17" t="n"/>
       <c r="AU33" s="16" t="n"/>
-      <c r="AV33" s="49" t="n"/>
-      <c r="AW33" s="56" t="n"/>
-      <c r="AX33" s="57" t="n"/>
-      <c r="AY33" s="20" t="n"/>
+      <c r="AV33" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AW33" t="inlineStr">
+        <is>
+          <t>9889.979</t>
+        </is>
+      </c>
+      <c r="AX33" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY33" s="5" t="n"/>
       <c r="AZ33" s="10" t="inlineStr">
         <is>
           <t>N</t>
@@ -7483,10 +7498,22 @@
       </c>
       <c r="AT34" s="18" t="n"/>
       <c r="AU34" s="13" t="n"/>
-      <c r="AV34" s="58" t="n"/>
-      <c r="AW34" s="59" t="n"/>
-      <c r="AX34" s="60" t="n"/>
-      <c r="AY34" s="20" t="n"/>
+      <c r="AV34" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="AW34" t="inlineStr">
+        <is>
+          <t>9977.973</t>
+        </is>
+      </c>
+      <c r="AX34" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY34" s="5" t="n"/>
       <c r="AZ34" s="10" t="inlineStr">
         <is>
           <t>E</t>
@@ -7615,10 +7642,22 @@
       </c>
       <c r="AT35" s="21" t="n"/>
       <c r="AU35" s="13" t="n"/>
-      <c r="AV35" s="53" t="n"/>
-      <c r="AW35" s="61" t="n"/>
-      <c r="AX35" s="62" t="n"/>
-      <c r="AY35" s="20" t="n"/>
+      <c r="AV35" t="inlineStr">
+        <is>
+          <t>EL</t>
+        </is>
+      </c>
+      <c r="AW35" t="inlineStr">
+        <is>
+          <t>17.405</t>
+        </is>
+      </c>
+      <c r="AX35" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY35" s="5" t="n"/>
       <c r="AZ35" s="11" t="inlineStr">
         <is>
           <t>EL</t>
@@ -7747,10 +7786,22 @@
       </c>
       <c r="AT36" s="17" t="n"/>
       <c r="AU36" s="23" t="n"/>
-      <c r="AV36" s="49" t="n"/>
-      <c r="AW36" s="56" t="n"/>
-      <c r="AX36" s="57" t="n"/>
-      <c r="AY36" s="20" t="n"/>
+      <c r="AV36" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="AW36" t="inlineStr">
+        <is>
+          <t>9889.979</t>
+        </is>
+      </c>
+      <c r="AX36" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY36" s="5" t="n"/>
       <c r="AZ36" s="10" t="inlineStr">
         <is>
           <t>N</t>
@@ -7879,10 +7930,22 @@
       </c>
       <c r="AT37" s="18" t="n"/>
       <c r="AU37" s="17" t="n"/>
-      <c r="AV37" s="58" t="n"/>
-      <c r="AW37" s="59" t="n"/>
-      <c r="AX37" s="60" t="n"/>
-      <c r="AY37" s="20" t="n"/>
+      <c r="AV37" t="inlineStr">
+        <is>
+          <t>E</t>
+        </is>
+      </c>
+      <c r="AW37" t="inlineStr">
+        <is>
+          <t>9977.973</t>
+        </is>
+      </c>
+      <c r="AX37" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY37" s="5" t="n"/>
       <c r="AZ37" s="10" t="inlineStr">
         <is>
           <t>E</t>
@@ -8011,10 +8074,22 @@
       </c>
       <c r="AT38" s="21" t="n"/>
       <c r="AU38" s="17" t="n"/>
-      <c r="AV38" s="53" t="n"/>
-      <c r="AW38" s="61" t="n"/>
-      <c r="AX38" s="62" t="n"/>
-      <c r="AY38" s="20" t="n"/>
+      <c r="AV38" t="inlineStr">
+        <is>
+          <t>EL</t>
+        </is>
+      </c>
+      <c r="AW38" t="inlineStr">
+        <is>
+          <t>17.405</t>
+        </is>
+      </c>
+      <c r="AX38" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="AY38" s="5" t="n"/>
       <c r="AZ38" s="11" t="inlineStr">
         <is>
           <t>EL</t>
@@ -8143,10 +8218,7 @@
       </c>
       <c r="AT39" s="17" t="n"/>
       <c r="AU39" s="16" t="n"/>
-      <c r="AV39" s="49" t="n"/>
-      <c r="AW39" s="56" t="n"/>
-      <c r="AX39" s="57" t="n"/>
-      <c r="AY39" s="20" t="n"/>
+      <c r="AY39" s="5" t="n"/>
       <c r="AZ39" s="10" t="inlineStr">
         <is>
           <t>N</t>
@@ -8275,10 +8347,7 @@
       </c>
       <c r="AT40" s="18" t="n"/>
       <c r="AU40" s="13" t="n"/>
-      <c r="AV40" s="58" t="n"/>
-      <c r="AW40" s="59" t="n"/>
-      <c r="AX40" s="60" t="n"/>
-      <c r="AY40" s="20" t="n"/>
+      <c r="AY40" s="5" t="n"/>
       <c r="AZ40" s="10" t="inlineStr">
         <is>
           <t>E</t>
@@ -8407,10 +8476,7 @@
       </c>
       <c r="AT41" s="21" t="n"/>
       <c r="AU41" s="22" t="n"/>
-      <c r="AV41" s="53" t="n"/>
-      <c r="AW41" s="61" t="n"/>
-      <c r="AX41" s="62" t="n"/>
-      <c r="AY41" s="20" t="n"/>
+      <c r="AY41" s="5" t="n"/>
       <c r="AZ41" s="11" t="inlineStr">
         <is>
           <t>EL</t>
@@ -8426,21 +8492,14 @@
       <c r="BD41" s="24" t="n"/>
     </row>
     <row r="42">
-      <c r="AW42" s="63" t="n"/>
-      <c r="AX42" s="63" t="n"/>
-      <c r="AY42" s="20" t="n"/>
+      <c r="AY42" s="5" t="n"/>
       <c r="BB42" s="5" t="n"/>
     </row>
     <row r="43">
-      <c r="AW43" s="63" t="n"/>
-      <c r="AX43" s="63" t="n"/>
-      <c r="AY43" s="20" t="n"/>
+      <c r="AY43" s="5" t="n"/>
       <c r="BB43" s="5" t="n"/>
     </row>
     <row r="44">
-      <c r="AW44" s="63" t="n"/>
-      <c r="AX44" s="63" t="n"/>
-      <c r="AY44" s="63" t="n"/>
       <c r="AZ44" s="28" t="inlineStr">
         <is>
           <t>Note: delta decimal feet</t>
@@ -12102,12 +12161,12 @@
       <c r="AU221" s="7" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="22">
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="AW2:AX2"/>
     <mergeCell ref="AZ1:BA1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="BC2:BD2"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="AB1:AC1"/>
@@ -12124,7 +12183,6 @@
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="AZ2:BA2"/>
-    <mergeCell ref="BC1:BD1"/>
     <mergeCell ref="AT1:AU1"/>
   </mergeCells>
   <pageMargins left="0.32" right="0.25" top="0.66" bottom="0.25" header="0.2" footer="0.25"/>

</xml_diff>